<commit_message>
last update night 09-02-2025 v2
</commit_message>
<xml_diff>
--- a/public/expenses.xlsx
+++ b/public/expenses.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="45">
   <si>
     <t>احتفالية معا نستطيع</t>
   </si>
@@ -106,9 +106,6 @@
     <t>عثمان اصالة - قناة السودان - كسلا</t>
   </si>
   <si>
-    <t>اعلام للمركز</t>
-  </si>
-  <si>
     <t>تراخيص المركز</t>
   </si>
   <si>
@@ -128,6 +125,30 @@
   </si>
   <si>
     <t xml:space="preserve">التاريخ </t>
+  </si>
+  <si>
+    <t>الضيافة</t>
+  </si>
+  <si>
+    <t>اطباق</t>
+  </si>
+  <si>
+    <t>ترحيل</t>
+  </si>
+  <si>
+    <t>ترحيل الاحتفال</t>
+  </si>
+  <si>
+    <t>تزين القاعة</t>
+  </si>
+  <si>
+    <t>20011907880 - 200119155061</t>
+  </si>
+  <si>
+    <t>البقالة</t>
+  </si>
+  <si>
+    <t>تجديد ترخيص ادارة التدريب الموحد</t>
   </si>
 </sst>
 </file>
@@ -582,10 +603,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O26"/>
+  <dimension ref="A1:O30"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:J23"/>
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -605,7 +626,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>2</v>
@@ -1146,7 +1167,7 @@
         <v>45667</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>14</v>
@@ -1172,7 +1193,7 @@
       </c>
       <c r="K16" s="7"/>
       <c r="O16" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
@@ -1183,7 +1204,7 @@
         <v>45667</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>14</v>
@@ -1209,7 +1230,7 @@
       </c>
       <c r="K17" s="7"/>
       <c r="O17" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
@@ -1220,7 +1241,7 @@
         <v>45667</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D18" s="7" t="s">
         <v>14</v>
@@ -1246,7 +1267,7 @@
       </c>
       <c r="K18" s="7"/>
       <c r="O18" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
@@ -1257,7 +1278,7 @@
         <v>45667</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>14</v>
@@ -1283,7 +1304,7 @@
       </c>
       <c r="K19" s="7"/>
       <c r="O19" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
@@ -1371,7 +1392,7 @@
         <v>12</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="E22" s="2">
         <v>1</v>
@@ -1386,7 +1407,7 @@
         <v>20</v>
       </c>
       <c r="I22" s="13">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J22" s="14">
         <f t="shared" si="0"/>
@@ -1402,70 +1423,213 @@
         <v>22</v>
       </c>
       <c r="B23" s="9">
-        <v>45652</v>
+        <v>45668</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="E23" s="2">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="F23" s="2">
-        <v>160000</v>
-      </c>
-      <c r="G23" s="3">
-        <v>20022963334</v>
-      </c>
-      <c r="H23" s="11" t="s">
+        <v>95000</v>
+      </c>
+      <c r="G23" s="2">
+        <v>20011928328</v>
+      </c>
+      <c r="H23" s="2" t="s">
         <v>20</v>
       </c>
       <c r="I23" s="13">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J23" s="14">
         <f t="shared" si="0"/>
-        <v>160000</v>
+        <v>2375</v>
       </c>
       <c r="K23" s="7"/>
       <c r="O23" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="7"/>
-      <c r="B24" s="9"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="11"/>
+      <c r="A24" s="7">
+        <v>23</v>
+      </c>
+      <c r="B24" s="9">
+        <v>45668</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E24" s="2">
+        <v>40</v>
+      </c>
+      <c r="F24" s="2">
+        <v>10000</v>
+      </c>
+      <c r="G24" s="2">
+        <v>20011892418</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I24" s="13">
+        <v>1</v>
+      </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="7"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="11"/>
+      <c r="A25" s="7">
+        <v>24</v>
+      </c>
+      <c r="B25" s="9">
+        <v>45668</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E25" s="2">
+        <v>1</v>
+      </c>
+      <c r="F25" s="2">
+        <v>7000</v>
+      </c>
+      <c r="G25" s="2">
+        <v>20011917072</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I25" s="13">
+        <v>3</v>
+      </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26" s="7"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
+      <c r="A26" s="7">
+        <v>25</v>
+      </c>
+      <c r="B26" s="9">
+        <v>45668</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E26" s="2">
+        <v>1</v>
+      </c>
       <c r="F26" s="2">
-        <f>SUM(F2:F25)</f>
-        <v>2565000</v>
-      </c>
-      <c r="G26" s="2"/>
-      <c r="H26" s="11"/>
+        <v>150000</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I26" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" s="7">
+        <v>26</v>
+      </c>
+      <c r="B27" s="9">
+        <v>45668</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E27" s="2">
+        <v>1</v>
+      </c>
+      <c r="F27" s="2">
+        <v>144000</v>
+      </c>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" s="7">
+        <v>27</v>
+      </c>
+      <c r="B28" s="9">
+        <v>45652</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E28" s="2">
+        <v>1</v>
+      </c>
+      <c r="F28" s="2">
+        <v>160000</v>
+      </c>
+      <c r="G28" s="2">
+        <v>20022963334</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I28" s="13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" s="7">
+        <v>28</v>
+      </c>
+      <c r="B29" s="9">
+        <v>45678</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E29" s="2">
+        <v>1</v>
+      </c>
+      <c r="F29" s="2">
+        <v>120000</v>
+      </c>
+      <c r="G29" s="2">
+        <v>20025165140</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I29" s="13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F30">
+        <f>SUM(F2:F29)</f>
+        <v>3091000</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
last update night 22-02-2025
</commit_message>
<xml_diff>
--- a/public/expenses.xlsx
+++ b/public/expenses.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="52">
   <si>
     <t>احتفالية معا نستطيع</t>
   </si>
@@ -149,13 +149,38 @@
   </si>
   <si>
     <t>تجديد ترخيص ادارة التدريب الموحد</t>
+  </si>
+  <si>
+    <t>نادي الشباب</t>
+  </si>
+  <si>
+    <t>صيانة المركز</t>
+  </si>
+  <si>
+    <t>الساوند قطية</t>
+  </si>
+  <si>
+    <t>ضيافة معا</t>
+  </si>
+  <si>
+    <t>لافتة معا الجديدة</t>
+  </si>
+  <si>
+    <t>ضيافه</t>
+  </si>
+  <si>
+    <t>صيانة</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -178,6 +203,14 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="178"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -254,10 +287,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -299,8 +333,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -603,10 +639,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O30"/>
+  <dimension ref="A1:O39"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1626,9 +1662,216 @@
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F30">
-        <f>SUM(F2:F29)</f>
-        <v>3091000</v>
+      <c r="A30" s="7">
+        <v>29</v>
+      </c>
+      <c r="B30" s="9">
+        <v>45666</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E30" s="7">
+        <v>1</v>
+      </c>
+      <c r="F30" s="7">
+        <v>1000000</v>
+      </c>
+      <c r="G30" s="7">
+        <v>20025846445</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" s="7">
+        <v>30</v>
+      </c>
+      <c r="B31" s="9">
+        <v>45666</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E31" s="7">
+        <v>1</v>
+      </c>
+      <c r="F31" s="7">
+        <v>10000</v>
+      </c>
+      <c r="G31" s="7">
+        <v>20024197699</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" s="7">
+        <v>31</v>
+      </c>
+      <c r="B32" s="9">
+        <v>45666</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E32" s="7">
+        <v>1</v>
+      </c>
+      <c r="F32" s="7">
+        <v>30000</v>
+      </c>
+      <c r="G32" s="7">
+        <v>20024244396</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="7">
+        <v>32</v>
+      </c>
+      <c r="B33" s="9">
+        <v>45666</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E33" s="7">
+        <v>1</v>
+      </c>
+      <c r="F33" s="7">
+        <v>120000</v>
+      </c>
+      <c r="G33" s="7">
+        <v>20024243209</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="7">
+        <v>33</v>
+      </c>
+      <c r="B34" s="9">
+        <v>45666</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E34" s="7">
+        <v>1</v>
+      </c>
+      <c r="F34" s="7">
+        <v>25000</v>
+      </c>
+      <c r="G34" s="7">
+        <v>20024244994</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="7">
+        <v>34</v>
+      </c>
+      <c r="B35" s="9">
+        <v>45666</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E35" s="7">
+        <v>1</v>
+      </c>
+      <c r="F35" s="7">
+        <v>330000</v>
+      </c>
+      <c r="G35" s="7">
+        <v>20024503051</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="7">
+        <v>35</v>
+      </c>
+      <c r="B36" s="9">
+        <v>45666</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E36" s="7">
+        <v>1</v>
+      </c>
+      <c r="F36" s="7">
+        <v>1000000</v>
+      </c>
+      <c r="G36" s="7">
+        <v>20023537607</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="7">
+        <v>36</v>
+      </c>
+      <c r="B37" s="9">
+        <v>45666</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E37" s="7">
+        <v>1</v>
+      </c>
+      <c r="F37" s="7">
+        <v>300000</v>
+      </c>
+      <c r="G37" s="7">
+        <v>20023647624</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="7">
+        <v>37</v>
+      </c>
+      <c r="B38" s="9">
+        <v>45666</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E38" s="7">
+        <v>1</v>
+      </c>
+      <c r="F38" s="7">
+        <v>500000</v>
+      </c>
+      <c r="G38" s="7">
+        <v>20023765391</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F39" s="15">
+        <f>SUM(F2:F38)</f>
+        <v>6406000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>